<commit_message>
update document and testcases
</commit_message>
<xml_diff>
--- a/test/testcases.xlsx
+++ b/test/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learning24\web\firstweb\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE81686-9C6C-4DE2-8370-BC28710AC5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A8EC87-7108-4D9F-992B-C1CCC654AFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1659,6 +1659,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1716,40 +1748,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -31202,17 +31202,17 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="90"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -31720,17 +31720,17 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="81"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="93"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -31794,17 +31794,17 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
       <c r="J16" s="5"/>
       <c r="K16" s="27"/>
       <c r="L16" s="5"/>
@@ -31868,17 +31868,17 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="85"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="97"/>
       <c r="J18" s="5"/>
       <c r="K18" s="27"/>
       <c r="L18" s="5"/>
@@ -59611,17 +59611,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="91"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="103"/>
     </row>
     <row r="3" spans="1:9" ht="73.5" customHeight="1">
       <c r="A3" s="66" t="s">
@@ -59925,17 +59925,17 @@
       <c r="I13" s="60"/>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="94"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="106"/>
     </row>
     <row r="15" spans="1:9" ht="266.39999999999998" customHeight="1">
       <c r="A15" s="58" t="s">
@@ -59965,17 +59965,17 @@
       <c r="I15" s="60"/>
     </row>
     <row r="16" spans="1:9" ht="17.399999999999999" customHeight="1">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="88"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="100"/>
     </row>
     <row r="17" spans="1:9" ht="117.6" customHeight="1">
       <c r="A17" s="58" t="s">
@@ -61018,7 +61018,7 @@
   <dimension ref="A1:I1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -61055,25 +61055,25 @@
       <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="83" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
     </row>
     <row r="3" spans="1:9" ht="98.25" customHeight="1" outlineLevel="1">
       <c r="A3" s="30" t="s">
@@ -61091,16 +61091,16 @@
       <c r="E3" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="106" t="s">
+      <c r="H3" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="107"/>
+      <c r="I3" s="86"/>
     </row>
     <row r="4" spans="1:9" ht="96.75" customHeight="1" outlineLevel="1">
       <c r="A4" s="33" t="s">
@@ -61124,10 +61124,10 @@
       <c r="G4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="98" t="s">
+      <c r="H4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="103"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="1:9" ht="109.5" customHeight="1" outlineLevel="1">
       <c r="A5" s="34" t="s">
@@ -61151,10 +61151,10 @@
       <c r="G5" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="103"/>
+      <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="153.75" customHeight="1" outlineLevel="1">
       <c r="A6" s="6" t="s">
@@ -61178,10 +61178,10 @@
       <c r="G6" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="103"/>
+      <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="153.75" customHeight="1" outlineLevel="1">
       <c r="A7" s="6" t="s">
@@ -61205,10 +61205,10 @@
       <c r="G7" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="103"/>
+      <c r="I7" s="82"/>
     </row>
     <row r="8" spans="1:9" ht="123.75" customHeight="1" outlineLevel="1">
       <c r="A8" s="6" t="s">
@@ -61232,10 +61232,10 @@
       <c r="G8" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="98" t="s">
+      <c r="H8" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="103"/>
+      <c r="I8" s="82"/>
     </row>
     <row r="9" spans="1:9" ht="110.25" customHeight="1" outlineLevel="1">
       <c r="A9" s="6" t="s">
@@ -61259,10 +61259,10 @@
       <c r="G9" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="100" t="s">
+      <c r="H9" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="109" t="s">
+      <c r="I9" s="87" t="s">
         <v>64</v>
       </c>
     </row>
@@ -61285,7 +61285,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="73"/>
-      <c r="I10" s="103"/>
+      <c r="I10" s="82"/>
     </row>
     <row r="11" spans="1:9" ht="97.5" customHeight="1" outlineLevel="1">
       <c r="A11" s="6" t="s">
@@ -61306,7 +61306,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="73"/>
-      <c r="I11" s="103"/>
+      <c r="I11" s="82"/>
     </row>
     <row r="12" spans="1:9" ht="90" customHeight="1" outlineLevel="1">
       <c r="A12" s="6" t="s">
@@ -61327,7 +61327,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="103"/>
+      <c r="I12" s="82"/>
     </row>
     <row r="13" spans="1:9" ht="90" customHeight="1" outlineLevel="1">
       <c r="A13" s="6" t="s">
@@ -61347,21 +61347,21 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="103"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="82"/>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="103"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="82"/>
     </row>
     <row r="15" spans="1:9" ht="114.75" customHeight="1">
       <c r="A15" s="75" t="s">
@@ -61381,8 +61381,8 @@
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="103"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
     </row>
     <row r="16" spans="1:9" ht="147" customHeight="1">
       <c r="A16" s="75" t="s">
@@ -61402,8 +61402,8 @@
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="103"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="82"/>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>